<commit_message>
updated xls and user manual
</commit_message>
<xml_diff>
--- a/GG V03 Testing_161122.xlsx
+++ b/GG V03 Testing_161122.xlsx
@@ -6337,12 +6337,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I15:I16"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>

</xml_diff>